<commit_message>
Read File Get Word Count Send to Excel (Date & Word Count)
</commit_message>
<xml_diff>
--- a/Example3.xlsx
+++ b/Example3.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,480 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>name3</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>address3</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>05/02/2022</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>name4</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>address4</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>tel4</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>web4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>